<commit_message>
Zwischencommiit Aspete 1 und 2 Projektbercht
</commit_message>
<xml_diff>
--- a/Planung/Planung.xlsx
+++ b/Planung/Planung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Woche</t>
   </si>
@@ -108,13 +108,16 @@
   </si>
   <si>
     <t>Diff</t>
+  </si>
+  <si>
+    <t>ABGABE Dokumentation/Anhänge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +129,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -310,6 +321,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -611,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,7 +714,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G23" si="0">F3-E3</f>
+        <f t="shared" ref="G3:G24" si="0">F3-E3</f>
         <v>-7</v>
       </c>
       <c r="H3" s="1"/>
@@ -756,7 +771,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>21</v>
       </c>
@@ -781,7 +796,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>22</v>
       </c>
@@ -1138,75 +1153,89 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
-        <f t="shared" si="0"/>
+        <f>F22-E22</f>
         <v>-18</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="17">
+        <v>41529</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
         <v>38</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B24" s="9">
         <v>41533</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="1">
-        <v>18</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1">
+      <c r="C24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="1">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
         <f t="shared" si="0"/>
         <v>-18</v>
       </c>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="1">
-        <f>SUM(E2:E23)</f>
+      <c r="D25" s="7"/>
+      <c r="E25" s="1">
+        <f>SUM(E2:E24)</f>
         <v>360</v>
       </c>
-      <c r="F24" s="1">
-        <f>SUM(F2:F23)</f>
+      <c r="F25" s="1">
+        <f>SUM(F2:F24)</f>
         <v>180.5</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <f>COUNT(A2:A23)</f>
-        <v>22</v>
-      </c>
-      <c r="B25" s="15">
-        <f>A25-2</f>
-        <v>20</v>
-      </c>
-      <c r="C25" s="16">
-        <f>360/B25</f>
-        <v>18</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1">
-        <f>AVERAGE(F2:F23)</f>
-        <v>16.40909090909091</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <f>COUNT(A2:A24)</f>
+        <v>22</v>
+      </c>
+      <c r="B26" s="15">
+        <f>A26-2</f>
+        <v>20</v>
+      </c>
+      <c r="C26" s="16">
+        <f>360/B26</f>
+        <v>18</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1">
+        <f>AVERAGE(F2:F24)</f>
+        <v>16.40909090909091</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Projektbericht und -handbuch für Review
</commit_message>
<xml_diff>
--- a/Planung/Planung.xlsx
+++ b/Planung/Planung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6180"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="25230" windowHeight="6120"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>Woche</t>
   </si>
@@ -31,9 +31,6 @@
 Kickoff Meeting vorbereiten</t>
   </si>
   <si>
-    <t>in Arbeit</t>
-  </si>
-  <si>
     <t>Ferien</t>
   </si>
   <si>
@@ -46,10 +43,6 @@
     <t>Stunden Aufwand pro Woche (360 h / Anzahl Wochen)</t>
   </si>
   <si>
-    <t>Auswertung bestehende Codebasis, Beurteilung wie kann was umgebaut werden,
-"Top-Aspekte" ermitteln und Strategie für Migration erarbeiten</t>
-  </si>
-  <si>
     <t>Sprint 1, Aspekt 1 angehen</t>
   </si>
   <si>
@@ -111,6 +104,9 @@
   </si>
   <si>
     <t>ABGABE Dokumentation/Anhänge</t>
+  </si>
+  <si>
+    <t>Aspektermittlung, Projekt-Setup</t>
   </si>
 </sst>
 </file>
@@ -628,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -657,16 +653,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -680,7 +676,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1">
         <v>18</v>
@@ -702,10 +698,10 @@
         <v>41393</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1">
         <v>18</v>
@@ -727,10 +723,10 @@
         <v>41400</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>18</v>
@@ -743,7 +739,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,10 +750,10 @@
         <v>41407</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1">
         <v>18</v>
@@ -771,7 +767,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>21</v>
       </c>
@@ -779,10 +775,10 @@
         <v>41414</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <v>18</v>
@@ -796,7 +792,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>22</v>
       </c>
@@ -804,10 +800,10 @@
         <v>41421</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="1">
         <v>18</v>
@@ -829,9 +825,11 @@
         <v>41428</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="1">
         <v>18</v>
       </c>
@@ -852,9 +850,11 @@
         <v>41435</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" s="1">
         <v>18</v>
       </c>
@@ -875,9 +875,11 @@
         <v>41442</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="1">
         <v>9</v>
       </c>
@@ -889,7 +891,7 @@
         <v>7</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -900,9 +902,11 @@
         <v>41449</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E11" s="1">
         <v>27</v>
       </c>
@@ -914,7 +918,7 @@
         <v>-10.5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,9 +929,11 @@
         <v>41456</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" s="1">
         <v>18</v>
       </c>
@@ -948,9 +954,11 @@
         <v>41463</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E13" s="1">
         <v>18</v>
       </c>
@@ -971,21 +979,23 @@
         <v>41470</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E14" s="1">
         <v>9</v>
       </c>
       <c r="F14" s="1">
-        <v>14.5</v>
+        <v>6.5</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>-2.5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -996,9 +1006,11 @@
         <v>41477</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E15" s="1">
         <v>27</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>-15</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1021,9 +1033,11 @@
         <v>41484</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E16" s="1">
         <v>18</v>
       </c>
@@ -1035,7 +1049,7 @@
         <v>3.5</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1046,9 +1060,11 @@
         <v>41491</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E17" s="1">
         <v>18</v>
       </c>
@@ -1069,9 +1085,11 @@
         <v>41498</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E18" s="1">
         <v>18</v>
       </c>
@@ -1092,9 +1110,9 @@
         <v>41505</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1">
         <v>0</v>
       </c>
@@ -1106,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1117,9 +1135,9 @@
         <v>41512</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1">
         <v>0</v>
       </c>
@@ -1139,9 +1157,9 @@
         <v>41519</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1">
         <v>18</v>
       </c>
@@ -1160,7 +1178,7 @@
         <v>41526</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="1">
@@ -1172,7 +1190,7 @@
         <v>-18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1181,7 +1199,7 @@
         <v>41529</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
@@ -1210,13 +1228,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="C25" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>8</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="1">
@@ -1225,11 +1243,11 @@
       </c>
       <c r="F25" s="1">
         <f>SUM(F2:F24)</f>
-        <v>319.5</v>
+        <v>311.5</v>
       </c>
       <c r="G25" s="1">
         <f>SUM(G2:G24)</f>
-        <v>-40.5</v>
+        <v>-48.5</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -1250,7 +1268,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1">
         <f>AVERAGE(F2:F24)</f>
-        <v>16.815789473684209</v>
+        <v>16.394736842105264</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>

</xml_diff>